<commit_message>
Update to research sheets
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Projects\Part-III-Individual-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\Projects\Part-III-Individual-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E33D7C-9309-4384-871D-D8D9B09B383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF47975-D48C-4B88-9B54-9D929E54FB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14370" yWindow="-24120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{4EC69FC7-84B9-4687-8CD2-1BF40196B0E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4EC69FC7-84B9-4687-8CD2-1BF40196B0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Data" sheetId="1" r:id="rId1"/>
     <sheet name="Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -270,18 +271,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C14A227-E12D-444E-9D9F-2891283F9C41}" name="Table1" displayName="Table1" ref="A1:I49" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C14A227-E12D-444E-9D9F-2891283F9C41}" name="Table1" displayName="Table1" ref="A1:I49" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:I49" xr:uid="{9C14A227-E12D-444E-9D9F-2891283F9C41}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5182EC7B-CEE5-4530-A3FE-7C3E89CF9D56}" name="Internal ID" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{26AE30E4-E47D-48DF-87F0-B76CECBA4893}" name="Referenced" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{0CF72881-A3BF-4F10-8D40-45329C2212E7}" name="Relevant?" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{15507EC0-7ABB-47B8-A469-4992E1223C04}" name="Year" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{57A9223A-8A9F-4F6E-BCB2-1EBF9632A0FC}" name="Author(s)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{5CF0D250-8F19-408D-B8D7-D423A692C9EA}" name="Title" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E135ABB2-4FC7-445F-8E7C-576A2F123182}" name="Resource Type" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{93CDDC6A-2383-48F0-B174-36C2A40A41A7}" name="Keywords" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{99F47420-97A0-4A4C-96BF-9D82FD6A3AFC}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{5182EC7B-CEE5-4530-A3FE-7C3E89CF9D56}" name="Internal ID" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{26AE30E4-E47D-48DF-87F0-B76CECBA4893}" name="Referenced" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{0CF72881-A3BF-4F10-8D40-45329C2212E7}" name="Relevant?" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{15507EC0-7ABB-47B8-A469-4992E1223C04}" name="Year" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{57A9223A-8A9F-4F6E-BCB2-1EBF9632A0FC}" name="Author(s)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{5CF0D250-8F19-408D-B8D7-D423A692C9EA}" name="Title" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E135ABB2-4FC7-445F-8E7C-576A2F123182}" name="Resource Type" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{93CDDC6A-2383-48F0-B174-36C2A40A41A7}" name="Keywords" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{99F47420-97A0-4A4C-96BF-9D82FD6A3AFC}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,21 +604,21 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.26953125" customWidth="1"/>
-    <col min="5" max="5" width="36.26953125" customWidth="1"/>
-    <col min="6" max="6" width="35.81640625" customWidth="1"/>
-    <col min="7" max="7" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="48.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="48.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -675,7 +676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -702,7 +703,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="114.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -727,7 +728,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="231.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -752,7 +753,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="141.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="141.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -763,7 +764,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -774,7 +775,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -785,7 +786,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -796,7 +797,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -807,7 +808,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -818,7 +819,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -829,7 +830,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -840,7 +841,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -851,7 +852,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -862,7 +863,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -873,7 +874,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -884,7 +885,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -895,7 +896,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -906,7 +907,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -917,7 +918,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -928,7 +929,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -939,7 +940,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -950,7 +951,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -961,7 +962,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -972,7 +973,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -983,7 +984,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -994,7 +995,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1005,7 +1006,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1016,7 +1017,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1027,7 +1028,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1038,7 +1039,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1049,7 +1050,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1060,7 +1061,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1071,7 +1072,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1082,7 +1083,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1093,7 +1094,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1104,7 +1105,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1115,7 +1116,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1126,7 +1127,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1137,7 +1138,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1148,7 +1149,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1159,7 +1160,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1170,7 +1171,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1181,7 +1182,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1192,7 +1193,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1203,7 +1204,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1214,7 +1215,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1225,7 +1226,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1236,7 +1237,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1245,7 +1246,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1254,7 +1255,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1263,7 +1264,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1272,7 +1273,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1281,7 +1282,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1290,7 +1291,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1299,7 +1300,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1308,7 +1309,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1317,7 +1318,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1326,7 +1327,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1335,7 +1336,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1344,7 +1345,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1353,7 +1354,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1362,7 +1363,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1371,7 +1372,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1380,7 +1381,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1389,7 +1390,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1412,18 +1413,18 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="106.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Add basic mathematical model example
</commit_message>
<xml_diff>
--- a/research.xlsx
+++ b/research.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\Projects\Part-III-Individual-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Projects\Part-III-Individual-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF47975-D48C-4B88-9B54-9D929E54FB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C364A1-F486-4A69-9216-B9235E1C64B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4EC69FC7-84B9-4687-8CD2-1BF40196B0E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4EC69FC7-84B9-4687-8CD2-1BF40196B0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Data" sheetId="1" r:id="rId1"/>
     <sheet name="Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Internal ID</t>
   </si>
@@ -167,6 +166,21 @@
   </si>
   <si>
     <t>Adaptive SIR model with vaccination: simultaneous identificiation of rates and functions illustrated with COVID-19</t>
+  </si>
+  <si>
+    <t>Modelling a Pandemic</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/modelling-a-pandemic-eb94025f248f</t>
+  </si>
+  <si>
+    <t>Christian Graf</t>
   </si>
 </sst>
 </file>
@@ -226,7 +240,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -271,18 +288,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C14A227-E12D-444E-9D9F-2891283F9C41}" name="Table1" displayName="Table1" ref="A1:I49" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:I49" xr:uid="{9C14A227-E12D-444E-9D9F-2891283F9C41}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5182EC7B-CEE5-4530-A3FE-7C3E89CF9D56}" name="Internal ID" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{26AE30E4-E47D-48DF-87F0-B76CECBA4893}" name="Referenced" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{0CF72881-A3BF-4F10-8D40-45329C2212E7}" name="Relevant?" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{15507EC0-7ABB-47B8-A469-4992E1223C04}" name="Year" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{57A9223A-8A9F-4F6E-BCB2-1EBF9632A0FC}" name="Author(s)" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5CF0D250-8F19-408D-B8D7-D423A692C9EA}" name="Title" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E135ABB2-4FC7-445F-8E7C-576A2F123182}" name="Resource Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{93CDDC6A-2383-48F0-B174-36C2A40A41A7}" name="Keywords" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{99F47420-97A0-4A4C-96BF-9D82FD6A3AFC}" name="Notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C14A227-E12D-444E-9D9F-2891283F9C41}" name="Table1" displayName="Table1" ref="A1:J49" totalsRowShown="0" dataDxfId="10">
+  <autoFilter ref="A1:J49" xr:uid="{9C14A227-E12D-444E-9D9F-2891283F9C41}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{5182EC7B-CEE5-4530-A3FE-7C3E89CF9D56}" name="Internal ID" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{26AE30E4-E47D-48DF-87F0-B76CECBA4893}" name="Referenced" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{0CF72881-A3BF-4F10-8D40-45329C2212E7}" name="Relevant?" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{15507EC0-7ABB-47B8-A469-4992E1223C04}" name="Year" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{57A9223A-8A9F-4F6E-BCB2-1EBF9632A0FC}" name="Author(s)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5CF0D250-8F19-408D-B8D7-D423A692C9EA}" name="Title" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E135ABB2-4FC7-445F-8E7C-576A2F123182}" name="Resource Type" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{93CDDC6A-2383-48F0-B174-36C2A40A41A7}" name="Keywords" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{99F47420-97A0-4A4C-96BF-9D82FD6A3AFC}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{7AFAF312-1805-4D9E-BF50-A0C84010CDB9}" name="URL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -598,27 +616,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C389DA9-DA3C-4B78-9FF4-F0E1F7F3972E}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" customWidth="1"/>
+    <col min="5" max="5" width="36.26953125" customWidth="1"/>
+    <col min="6" max="6" width="35.81640625" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="48.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="48.54296875" customWidth="1"/>
+    <col min="10" max="10" width="33.36328125" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,8 +665,11 @@
       <c r="I1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -675,8 +697,9 @@
       <c r="I2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -702,8 +725,9 @@
         <v>13</v>
       </c>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="114.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -727,8 +751,9 @@
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="231.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="232" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -752,19 +777,33 @@
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="141.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="141.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="D6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -774,8 +813,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -785,8 +825,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -796,8 +837,9 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -807,8 +849,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -818,8 +861,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -829,8 +873,9 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -840,8 +885,9 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -851,8 +897,9 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -862,8 +909,9 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -873,8 +921,9 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -884,8 +933,9 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -895,8 +945,9 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -906,8 +957,9 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -917,8 +969,9 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -928,8 +981,9 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -939,8 +993,9 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -950,8 +1005,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -961,8 +1017,9 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -972,8 +1029,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -983,8 +1041,9 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -994,8 +1053,9 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1005,8 +1065,9 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1016,8 +1077,9 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1027,8 +1089,9 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1038,8 +1101,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1049,8 +1113,9 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1060,8 +1125,9 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1071,8 +1137,9 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1082,8 +1149,9 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1093,8 +1161,9 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1104,8 +1173,9 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1115,8 +1185,9 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1126,8 +1197,9 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1137,8 +1209,9 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1148,8 +1221,9 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1159,8 +1233,9 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1170,8 +1245,9 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1181,8 +1257,9 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1192,8 +1269,9 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1203,8 +1281,9 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1214,8 +1293,9 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1225,8 +1305,9 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1236,8 +1317,9 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1246,7 +1328,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1255,7 +1337,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1264,7 +1346,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1273,7 +1355,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1282,7 +1364,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1291,7 +1373,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1300,7 +1382,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1309,7 +1391,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1318,7 +1400,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1327,7 +1409,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1336,7 +1418,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1345,7 +1427,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1354,7 +1436,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1363,7 +1445,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1372,7 +1454,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1381,7 +1463,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1390,7 +1472,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1412,19 +1494,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB8522A-5968-44E1-82FE-25FEA4870976}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="106.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1438,7 +1520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1449,7 +1531,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1463,7 +1545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1477,7 +1559,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>

</xml_diff>